<commit_message>
Más datos de Oscar
</commit_message>
<xml_diff>
--- a/excel/OscarData.xlsx
+++ b/excel/OscarData.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oscardp96/Development/TID_PROYECTO/Datos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oscardp96/Development/TID_PROYECTO/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23120" windowHeight="21600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="869" uniqueCount="52">
   <si>
     <t>Lugar de Partida</t>
   </si>
@@ -129,13 +129,67 @@
   </si>
   <si>
     <t>La Cuesta</t>
+  </si>
+  <si>
+    <t>Ravelo</t>
+  </si>
+  <si>
+    <t>El Ortigal</t>
+  </si>
+  <si>
+    <t>8.5</t>
+  </si>
+  <si>
+    <t>Montaña</t>
+  </si>
+  <si>
+    <t>Las Carboneras</t>
+  </si>
+  <si>
+    <t>Las Mercedes</t>
+  </si>
+  <si>
+    <t>11.4</t>
+  </si>
+  <si>
+    <t>Parque La Granja</t>
+  </si>
+  <si>
+    <t>La Verdellada</t>
+  </si>
+  <si>
+    <t>4.1</t>
+  </si>
+  <si>
+    <t>Ciudad</t>
+  </si>
+  <si>
+    <t>Campus central ULL</t>
+  </si>
+  <si>
+    <t>3.2</t>
+  </si>
+  <si>
+    <t>Plaza Weyler</t>
+  </si>
+  <si>
+    <t>Hotel Mencey</t>
+  </si>
+  <si>
+    <t>La Villa</t>
+  </si>
+  <si>
+    <t>San Antonio (Orotava)</t>
+  </si>
+  <si>
+    <t>4.8</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -147,6 +201,29 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -190,10 +267,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -201,8 +296,29 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="19">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -478,10 +594,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K50"/>
+  <dimension ref="A1:K92"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2249,6 +2365,1476 @@
         <v>33</v>
       </c>
     </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I51" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J51" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K51" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A52" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I52" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J52" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K52" s="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I53" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J53" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K53" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H54" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I54" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J54" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K54" s="1">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A55" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H55" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I55" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J55" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K55" s="1">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A56" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F56" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G56" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H56" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I56" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J56" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="K56" s="3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A57" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F57" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G57" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H57" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I57" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J57" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="K57" s="3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A58" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H58" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I58" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J58" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K58" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A59" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H59" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I59" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J59" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K59" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A60" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F60" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G60" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H60" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I60" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J60" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K60" s="3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A61" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F61" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G61" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H61" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I61" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J61" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K61" s="3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A62" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H62" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I62" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J62" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K62" s="1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A63" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F63" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G63" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H63" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I63" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J63" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K63" s="3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A64" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F64" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G64" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H64" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I64" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J64" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K64" s="3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A65" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F65" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G65" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H65" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I65" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J65" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K65" s="3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A66" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F66" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G66" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H66" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I66" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J66" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K66" s="3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A67" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E67" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F67" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G67" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H67" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I67" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J67" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K67" s="3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A68" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E68" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F68" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G68" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H68" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I68" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J68" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K68" s="3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A69" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E69" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F69" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G69" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H69" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I69" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J69" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K69" s="3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A70" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F70" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G70" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H70" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I70" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J70" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K70" s="3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A71" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E71" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F71" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G71" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H71" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I71" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J71" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K71" s="3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A72" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G72" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H72" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I72" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J72" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K72" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A73" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G73" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H73" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I73" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J73" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K73" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A74" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G74" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H74" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I74" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J74" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K74" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A75" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G75" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H75" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I75" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J75" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K75" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A76" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G76" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H76" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I76" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J76" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K76" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A77" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G77" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H77" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I77" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J77" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K77" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A78" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C78" s="1">
+        <v>1</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G78" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H78" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I78" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J78" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K78" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A79" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C79" s="1">
+        <v>1</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G79" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H79" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I79" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J79" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K79" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A80" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C80" s="1">
+        <v>1</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G80" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H80" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I80" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J80" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K80" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A81" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G81" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H81" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I81" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J81" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K81" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A82" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G82" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H82" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I82" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J82" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K82" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A83" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G83" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H83" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I83" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J83" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K83" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A84" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D84" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E84" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F84" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G84" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H84" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I84" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J84" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K84" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A85" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D85" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E85" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F85" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G85" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H85" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I85" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J85" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K85" s="3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A86" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D86" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E86" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F86" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G86" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H86" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I86" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J86" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K86" s="3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A87" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D87" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E87" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F87" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G87" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H87" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I87" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J87" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K87" s="3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A88" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C88" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D88" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E88" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F88" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G88" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H88" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I88" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J88" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K88" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A89" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D89" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E89" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F89" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G89" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H89" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I89" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J89" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K89" s="3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A90" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D90" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E90" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F90" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G90" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H90" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I90" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J90" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K90" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A91" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B91" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C91" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D91" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E91" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F91" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G91" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H91" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I91" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J91" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K91" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A92" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C92" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D92" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E92" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F92" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G92" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H92" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I92" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J92" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K92" s="3">
+        <v>46</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>